<commit_message>
test cases are updated
</commit_message>
<xml_diff>
--- a/src/test/resources/DataFile.xlsx
+++ b/src/test/resources/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandanpanigrahi/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandanpanigrahi/Documents/Automation Frameworks_Eclipse/PlaywrightUI/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB8282-89AA-5D42-B857-861217DD6E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDB16CE-0323-8E4F-8C0E-6C31FF1FE4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{E1572F0D-6232-0C45-A66A-ABBC6DC64D86}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15640" xr2:uid="{E1572F0D-6232-0C45-A66A-ABBC6DC64D86}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -44,47 +44,50 @@
     <t>password</t>
   </si>
   <si>
-    <t>chandan</t>
+    <t>widentechinfo@gmail.com</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Akash</t>
-  </si>
-  <si>
-    <t>Abhash</t>
-  </si>
-  <si>
-    <t>Pritish</t>
-  </si>
-  <si>
-    <t>Ravi</t>
-  </si>
-  <si>
-    <t>Sid</t>
-  </si>
-  <si>
-    <t>Chandini</t>
-  </si>
-  <si>
-    <t>Chinu</t>
-  </si>
-  <si>
-    <t>Lipsa</t>
+    <t>techinfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Candara"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="20"/>
+      <color theme="10"/>
+      <name val="Candara"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Candara"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,13 +107,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,95 +451,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4FA4CF-C191-BE45-B8AD-ACE3E3DF1FB2}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FF7B6D7F-730D-5043-A68B-01C18BEEA4EC}"/>
+    <hyperlink ref="A3:A7" r:id="rId2" display="widentechinfo@gmail.com" xr:uid="{7857395F-CCD8-3844-9E74-EEEF0FF06714}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>